<commit_message>
code 1811 - 09
</commit_message>
<xml_diff>
--- a/ui/data/test_add_address.xlsx
+++ b/ui/data/test_add_address.xlsx
@@ -8,18 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
-  <si>
-    <t>sno</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>yes</t>
   </si>
@@ -63,9 +60,6 @@
     <t>aus</t>
   </si>
   <si>
-    <t>Flag</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -79,6 +73,12 @@
   </si>
   <si>
     <t>Zip</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Sno</t>
   </si>
 </sst>
 </file>
@@ -455,25 +455,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -484,16 +484,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1">
         <v>500018</v>
@@ -504,19 +504,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1">
         <v>500019</v>
@@ -526,20 +526,18 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
         <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1">
         <v>500020</v>
@@ -550,19 +548,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1">
         <v>500021</v>

</xml_diff>